<commit_message>
fixed recordJSONResponse, added basic check to date input, renamed hh_tide_values to tide_values
</commit_message>
<xml_diff>
--- a/Spring_High_Data.xlsx
+++ b/Spring_High_Data.xlsx
@@ -469,8 +469,8 @@
           <t>20240324</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>7.474</v>
+      <c r="B3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -479,8 +479,8 @@
           <t>20240408</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>5</v>
+      <c r="B4" s="2" t="n">
+        <v>7.044</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>7.044</v>
+        <v>5.82</v>
       </c>
     </row>
     <row r="6">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>5.82</v>
+        <v>6.434</v>
       </c>
     </row>
     <row r="7">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>6.434</v>
+        <v>5.981</v>
       </c>
     </row>
     <row r="8">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>5.981</v>
+        <v>6.496</v>
       </c>
     </row>
     <row r="9">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>6.496</v>
+        <v>4.078</v>
       </c>
     </row>
     <row r="10">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>5.974</v>
+        <v>6.191</v>
       </c>
     </row>
     <row r="14">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>6.155</v>
+        <v>5.974</v>
       </c>
     </row>
     <row r="15">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>6.283</v>
+        <v>5.951</v>
       </c>
     </row>
     <row r="16">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>6.49</v>
+        <v>6.155</v>
       </c>
     </row>
     <row r="17">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>5.256</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="18">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>7.543</v>
+        <v>5.256</v>
       </c>
     </row>
     <row r="19">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>4.734</v>
+        <v>7.543</v>
       </c>
     </row>
     <row r="20">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>5.745</v>
+        <v>4.734</v>
       </c>
     </row>
     <row r="21">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>6.217</v>
+        <v>5.745</v>
       </c>
     </row>
     <row r="22">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>6.155</v>
+        <v>6.217</v>
       </c>
     </row>
     <row r="23">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>5.581</v>
+        <v>6.155</v>
       </c>
     </row>
     <row r="24">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>5.945</v>
+        <v>5.581</v>
       </c>
     </row>
     <row r="25">
@@ -690,10 +690,19 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
+        <v>5.945</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20250227</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
         <v>6.512</v>
       </c>
     </row>
-    <row r="26"/>
     <row r="27"/>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
@@ -702,7 +711,7 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>6.127000000000001</v>
+        <v>6.009</v>
       </c>
     </row>
     <row r="29">
@@ -712,7 +721,7 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>6.194125</v>
+        <v>6.044880000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the api to call for the spring moon date as well as the next day ; changed the recordJSONResponse to look at all entries and take the highest of them rather than the first listed as HH
</commit_message>
<xml_diff>
--- a/Spring_High_Data.xlsx
+++ b/Spring_High_Data.xlsx
@@ -469,8 +469,8 @@
           <t>20240324</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>5</v>
+      <c r="B3" s="2" t="n">
+        <v>5.768</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>7.044</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>5.82</v>
+        <v>6.106</v>
       </c>
     </row>
     <row r="6">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>6.434</v>
+        <v>6.762</v>
       </c>
     </row>
     <row r="7">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>5.981</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="8">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>6.496</v>
+        <v>6.749</v>
       </c>
     </row>
     <row r="9">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>4.078</v>
+        <v>5.732</v>
       </c>
     </row>
     <row r="10">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>6.099</v>
+        <v>6.342</v>
       </c>
     </row>
     <row r="11">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.037</v>
+        <v>6.112</v>
       </c>
     </row>
     <row r="12">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.191</v>
+        <v>6.985</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>5.951</v>
+        <v>6.588</v>
       </c>
     </row>
     <row r="16">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>6.155</v>
+        <v>6.283</v>
       </c>
     </row>
     <row r="17">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>6.49</v>
+        <v>7.149</v>
       </c>
     </row>
     <row r="18">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>4.734</v>
+        <v>5.089</v>
       </c>
     </row>
     <row r="21">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>5.745</v>
+        <v>6.352</v>
       </c>
     </row>
     <row r="22">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>5.945</v>
+        <v>6.739</v>
       </c>
     </row>
     <row r="26">
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>6.009</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="29">
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>6.044880000000001</v>
+        <v>6.351520000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added output for text GUI - no functionality yet
added an output for what I would like the text GUI to look like in the printMainMenu function, and also changed all instances of 'average' to mean for specificity purposes.
</commit_message>
<xml_diff>
--- a/Spring_High_Data.xlsx
+++ b/Spring_High_Data.xlsx
@@ -456,251 +456,251 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20240310</t>
+          <t>20000106</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>8.002000000000001</v>
+        <v>4.905</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20240324</t>
+          <t>20000120</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5.768</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20240408</t>
+          <t>20000205</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>7.1</v>
+        <v>4.836</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20240423</t>
+          <t>20000219</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>6.106</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20240507</t>
+          <t>20000305</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>6.762</v>
+        <v>5.276</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20240523</t>
+          <t>20000319</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>6.01</v>
+        <v>6.178</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20240606</t>
+          <t>20000404</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>6.749</v>
+        <v>5.522</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20240621</t>
+          <t>20000418</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>5.732</v>
+        <v>6.657</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20240705</t>
+          <t>20000503</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>6.342</v>
+        <v>5.594</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20240721</t>
+          <t>20000517</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.112</v>
+        <v>5.538</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20240804</t>
+          <t>20000602</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>5.682</v>
+        <v>6.325</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20240819</t>
+          <t>20000616</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>6.985</v>
+        <v>5.476</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20240902</t>
+          <t>20000701</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>5.974</v>
+        <v>6.306</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20240917</t>
+          <t>20000716</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>6.588</v>
+        <v>5.666</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20241002</t>
+          <t>20000730</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>6.283</v>
+        <v>6.424</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20241017</t>
+          <t>20000814</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>7.149</v>
+        <v>6.037</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20241031</t>
+          <t>20000829</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>5.256</v>
+        <v>6.447</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20241115</t>
+          <t>20000913</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>7.543</v>
+        <v>5.446</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20241130</t>
+          <t>20000927</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>5.089</v>
+        <v>6.841</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20241215</t>
+          <t>20001013</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>6.352</v>
+        <v>5.331</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20241230</t>
+          <t>20001027</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>6.217</v>
+        <v>6.066</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20250113</t>
+          <t>20001111</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>6.155</v>
+        <v>6.526</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20250129</t>
+          <t>20001125</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>5.581</v>
+        <v>6.759</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20250212</t>
+          <t>20001211</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>6.739</v>
+        <v>6.375</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20250227</t>
+          <t>20001225</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>6.512</v>
+        <v>4.747</v>
       </c>
     </row>
     <row r="27"/>
@@ -711,17 +711,17 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>6.25</v>
+        <v>6.0435</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>Average:</t>
+          <t>mean:</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>6.351520000000002</v>
+        <v>5.91952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>